<commit_message>
Jan 27th: Room Commands Feedback
</commit_message>
<xml_diff>
--- a/New_John_EMS_Module_Library_TCP/TCP Info/TCP Putty Test Cases.xlsx
+++ b/New_John_EMS_Module_Library_TCP/TCP Info/TCP Putty Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\New_John_EMS_Module_Library_TCP\TCP Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A9A0CE-F56C-47BB-91BB-7ECC94C43DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0094EE3A-09D5-4794-9A45-DED50799F208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6910" yWindow="1130" windowWidth="23940" windowHeight="19390" xr2:uid="{117AF618-641C-4A92-974A-9DF04D6D90EC}"/>
+    <workbookView xWindow="7850" yWindow="2990" windowWidth="24800" windowHeight="16930" xr2:uid="{117AF618-641C-4A92-974A-9DF04D6D90EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="121">
   <si>
     <t>CAMERA</t>
   </si>
@@ -135,9 +135,6 @@
   </si>
   <si>
     <t>Leave Privacy</t>
-  </si>
-  <si>
-    <t>{[Room][Status][RM01][1]}</t>
   </si>
   <si>
     <t>{[Room][Status][RM01][2]}</t>
@@ -200,9 +197,6 @@
 * We already have paging route and room mute, but here we're requesting the status of these.</t>
   </si>
   <si>
-    <t>The Scheduler in TCP sheet is the EMS SW!</t>
-  </si>
-  <si>
     <t>PAGING one way.  SW tells Crestron to Page!  IF the Crestron/TP user
 clicks Paging, that's sent to Biamp, but not Crestron!</t>
   </si>
@@ -259,20 +253,6 @@
   </si>
   <si>
     <t>{[Paging][Route][6][0]}</t>
-  </si>
-  <si>
-    <t>*mutes ceiling mic in the room. Since this goes to the camera.
-  (The room speaker doesn't). Corresponds to Room</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TO DO
--feedback is set for both directions by storing data in the Room object both ways, BUT still need to highlight button both ways.
--Minish 1- Yes, we can't do recording when Privacy is enable.    2- Yes, recording will continue, their is no effect on recording.  currently this is the functionality we have.  But In 2nd query we can pop up a message for end user and say that recording is going on privacy won't work.
--Need error checking for people passing wrong commands
--Put set state in front of the ack. If set state failes then you don't ack back. Room commands.
-NOTES
-*So, Room Mute,mic.  1 per room.   Think these depend on Biamp values, but John has it so room1 uses Mute_1 instance.
-*The Crestron tells SW to record room.  The SW DOES tell Crestron it has recorded the room in the form of fb, if room recorded, tell Crestron so it can highlight the button.  </t>
   </si>
   <si>
     <t>{[Paging][Clear][6][6]}</t>
@@ -382,23 +362,122 @@
     <t>REQUEST</t>
   </si>
   <si>
-    <t>{[Request][Status][1,2]}
-{[ACK][Status][room 1][status value],[ACK][Status][room 2][status value]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status: {[Request][Status][0]}
-{[ACK][Status][room 1][status value],[ACK][Status][room 2][status value]}
+    <t>All Rooms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{[Request][Status][0]}
+{[ACK][Status][RM01][status value],[ACK][Status][RM02][status value]}
 </t>
   </si>
   <si>
-    <t>All Rooms</t>
+    <t xml:space="preserve">Status: {[Request][Privacy][0]}
+{[ACK][Privacy][RM01][status value],[ACK][Privacy][RM02][status value]}
+</t>
+  </si>
+  <si>
+    <t>{[Request][Status][RM01,RM02]}
+{[ACK][Status][RM01][status value],[ACK][Status][RM02][status value]}</t>
+  </si>
+  <si>
+    <t>{[Request][Privacy][RM01,RM02]}
+{[ACK][Status][RM01][status value],[ACK][Privacy][RM02][status value]}</t>
+  </si>
+  <si>
+    <t>** DOES THIS REQUEST come from the TP.  Or just console
+command, because user would have to pick a handful of rooms
+at once to get status on.
+*Also, I guess the results would update our feedback?</t>
+  </si>
+  <si>
+    <t>WAIT THIS IS NOT NEEDED??</t>
+  </si>
+  <si>
+    <t>{[Request][Mute][RM01,RM02]}
+{[ACK][Mute][RM01][status value],[ACK][Mute][RM02][status value]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{[Request][Mute][0]}
+{[ACK][Mute][RM01][status value],[ACK][Mute][RM02][status value]}
+</t>
+  </si>
+  <si>
+    <t>***</t>
+  </si>
+  <si>
+    <t>If Hercules Server NOT WORKING:
+*Hercules not working: run terminal: ncat -k -l 53125 to start port in terminal
+*Then, GET the ID number, netstat -aon | findstr :53125
+*Then, end the port: taskkill /PID 16408 /F</t>
+  </si>
+  <si>
+    <t>{[Request][Route][6]}
+{[ACK][Route][6][6,7]}</t>
+  </si>
+  <si>
+    <t>* Currently this state of things is not held in array, but rather by the button being lit up. THIS OK?
+* Also, do I need to use the Biamp ACK, as the way the FB needs to be updated.</t>
+  </si>
+  <si>
+    <t>USE LIVE FB EVERYWHERE.  NOT EMULATED!
+IF SW TELLS US, we trust that as live.  But everything else like having to route
+and mute get it from the Biamp</t>
+  </si>
+  <si>
+    <t>Pause Recording; Multi Rooms</t>
+  </si>
+  <si>
+    <t>TO DO
+-When EMS SW reaches out to us, we don’t ACK something is working till we get the ACK from the Biamp. This Always the case!
+NOTES
+*mutes ceiling mic in the room. Since this goes to the camera.
+  (The room speaker doesn't). Corresponds to Room</t>
+  </si>
+  <si>
+    <t>Room Control TP-&gt;Crestron Client-&gt;EMS SW Server [Hercules] -&gt; ACKs to Crestron Client</t>
+  </si>
+  <si>
+    <t>Stop Recording; MultiRooms</t>
+  </si>
+  <si>
+    <t>Start Recording; MultiRooms; ACK back we're in privacy mode</t>
+  </si>
+  <si>
+    <t>{[Room][Status][RM01,RM02][1]}
+{[ACK][Status][RM01][5], [ACK][Status][RM02][5]}</t>
+  </si>
+  <si>
+    <t>{[Room][Status][RM01][1]}
+{[ACK][Status][RM01][1]}</t>
+  </si>
+  <si>
+    <t>{[Room][Status][RM01,RM02][2]}
+{[ACK][Status][RM01][2],[ACK][Status][RM02][2]}</t>
+  </si>
+  <si>
+    <t>{[Room][Status][RM01,RM02][3]}
+{[ACK][Status][RM01][3],[ACK][Status][RM02][3]}</t>
+  </si>
+  <si>
+    <t>* Yes, we get the correct ACKS for all this too!</t>
+  </si>
+  <si>
+    <t>TO DO
+-Minish 1- Yes, we can't do recording when Privacy is enable.    2- Yes, recording will continue, their is no effect on recording.  currently this is the functionality we have.  But In 2nd query we can pop up a message for end user and say that recording is going on privacy won't work.
+-Need error checking for people passing wrong commands
+NOTES
+*So, Room Mute,mic.  1 per room.   Think these depend on Biamp values, but John has it so room1 uses Mute_1 instance.
+*The Crestron tells SW to record room.  The SW DOES tell Crestron it has recorded the room in the form of fb, if room recorded, tell Crestron so it can highlight the button.  
+Johns prot corect, sw determines logic.  Cause they are closer to weather we are in privacy mode or not. So all this recording on privacy logic i think will be with them.</t>
+  </si>
+  <si>
+    <t>*we call biamp, then from TP. Ack from them means update. Like paging, I don't think we need to tell EMS SW we did this</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,8 +528,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -499,6 +600,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2485C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -512,7 +625,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -533,19 +646,35 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -887,17 +1016,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F8A7121-B9AA-4E0E-9B0F-4628FA59633E}">
-  <dimension ref="A1:C99"/>
+  <dimension ref="A1:C124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="83.1796875" customWidth="1"/>
     <col min="2" max="2" width="67.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.81640625" customWidth="1"/>
+    <col min="3" max="3" width="61.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
@@ -911,130 +1040,135 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" ht="60.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+    </row>
+    <row r="3" spans="1:3" s="24" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="C4" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B6" s="7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B10" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B12" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B13" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B12" s="7"/>
-      <c r="C12" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B14" s="7"/>
+      <c r="C14" s="10"/>
+    </row>
+    <row r="15" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B15" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C14" s="10"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C15" s="10"/>
+      <c r="C15" s="11" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C16" s="10"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+      <c r="C17" s="10"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C18" s="10"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="10"/>
-    </row>
-    <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="C19" s="10"/>
+    </row>
+    <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="10"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B19" s="8"/>
-      <c r="C19" s="10"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="6"/>
+      <c r="B20" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="C20" s="10"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B21" s="8"/>
       <c r="C21" s="10"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>3</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B22" s="6"/>
       <c r="C22" s="10"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -1042,7 +1176,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C24" s="10"/>
     </row>
@@ -1051,428 +1185,533 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="10"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C27" s="10"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="10"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="5" t="s">
+      <c r="C28" s="10"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="261" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
+    <row r="37" spans="1:3" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+      <c r="C37" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>28</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C38" s="12"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>30</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B39" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="C39" s="7"/>
+    </row>
+    <row r="40" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>31</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+      <c r="B40" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40" s="7"/>
+    </row>
+    <row r="41" spans="1:3" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>32</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+      <c r="B41" s="28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B42" s="28"/>
+      <c r="C42" s="7"/>
+    </row>
+    <row r="43" spans="1:3" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>49</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B43" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="C43" s="7"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B44" s="7"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B45" s="15"/>
-    </row>
-    <row r="46" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
-        <v>28</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C46" s="7"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>29</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>30</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
+      <c r="B45" s="7"/>
+    </row>
+    <row r="46" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="47" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="48" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>31</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
+      </c>
+      <c r="B49" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" s="31" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>32</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
+      </c>
+      <c r="B50" s="30" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
+        <v>31</v>
+      </c>
+      <c r="B51" s="30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>32</v>
+      </c>
+      <c r="B52" s="30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>45</v>
+      </c>
+      <c r="B53" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="C53" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>47</v>
+      </c>
+      <c r="B54" s="29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" s="14"/>
+    </row>
+    <row r="57" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>28</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C57" s="7"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>29</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>31</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>32</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>45</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>47</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="13"/>
+      <c r="B65" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="13"/>
+      <c r="B66" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="13" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>48</v>
-      </c>
-      <c r="B52" s="6" t="s">
+      <c r="B67" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B69" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B70" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="14.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="73" spans="1:3" ht="319" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="14"/>
-      <c r="B54" s="6" t="s">
+    <row r="75" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A75" s="13" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="14"/>
-      <c r="B55" s="6" t="s">
+      <c r="B75" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="14" t="s">
+      <c r="B76" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C76" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="6" t="s">
+      <c r="B77" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C77" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>55</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79" s="15" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" ht="14.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="62" spans="1:3" ht="333.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C62" s="4" t="s">
+      <c r="B79" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>62</v>
+      </c>
+      <c r="B80" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>62</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>57</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>55</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>83</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>84</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>85</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>86</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>87</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>88</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>89</v>
+      </c>
+      <c r="B92" s="16"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>90</v>
+      </c>
+      <c r="B93" s="17"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B94" s="18"/>
+    </row>
+    <row r="96" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A96" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A101" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A102" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B102" s="19"/>
+      <c r="C102" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A103" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B103" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C103" s="21"/>
+    </row>
+    <row r="104" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A104" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B104" s="21" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A63" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A64" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C65" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A66" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C66" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A69" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B69" s="18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A70" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A71" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A72" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A73" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A74" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A75" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="B75" s="6" t="s">
+      <c r="C104" s="19"/>
+    </row>
+    <row r="105" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A105" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B105" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C105" s="19"/>
+    </row>
+    <row r="106" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A106" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B106" s="21" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A76" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="B76" s="6" t="s">
+      <c r="C106" s="19"/>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A107" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B107" s="19"/>
+      <c r="C107" s="19"/>
+    </row>
+    <row r="108" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A108" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B108" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A77" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A78" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A79" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="B79" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A80" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="B81" s="18"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A82" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="B82" s="19"/>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" s="16"/>
-      <c r="B83" s="20"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A84" s="16"/>
-    </row>
-    <row r="85" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A85" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C85" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A90" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A91" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A92" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B92" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C92" s="21"/>
-    </row>
-    <row r="93" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
-        <v>101</v>
-      </c>
-      <c r="B93" s="9" t="s">
+      <c r="B109" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A110" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A115" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C115" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A98" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C98" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
+    <row r="123" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A123" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C123" s="4" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>